<commit_message>
cas general affichage dynamique
</commit_message>
<xml_diff>
--- a/DataSeating.xlsx
+++ b/DataSeating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/690ee0af85bd39dc/Documents/cs/st7 - opti transport/Projet-avion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9962ABD-297F-4C7F-9B89-B890AB52DC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{A9962ABD-297F-4C7F-9B89-B890AB52DC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B314B504-714D-4B85-8A58-A91B049EFB7D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="21Oct" sheetId="1" r:id="rId1"/>
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A112"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2431,11 +2431,11 @@
       <c r="A108" s="3">
         <v>107</v>
       </c>
-      <c r="B108" s="4">
-        <v>1</v>
-      </c>
+      <c r="B108" s="4"/>
       <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
+      <c r="D108" s="4">
+        <v>1</v>
+      </c>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
       <c r="G108" s="4" t="s">
@@ -2489,7 +2489,9 @@
         <v>2</v>
       </c>
       <c r="C111" s="4"/>
-      <c r="D111" s="4"/>
+      <c r="D111" s="4">
+        <v>1</v>
+      </c>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
       <c r="G111" s="4" t="s">
@@ -2507,7 +2509,9 @@
       <c r="C112" s="4">
         <v>1</v>
       </c>
-      <c r="D112" s="4"/>
+      <c r="D112" s="4">
+        <v>1</v>
+      </c>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
       <c r="G112" s="4" t="s">
@@ -2521,7 +2525,7 @@
       <c r="A113" s="3"/>
       <c r="B113" s="4">
         <f>SUM(B2:B112)</f>
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C113" s="4">
         <f t="shared" ref="C113:E113" si="0">SUM(C2:C112)</f>
@@ -2529,7 +2533,7 @@
       </c>
       <c r="D113" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E113" s="4">
         <f t="shared" si="0"/>
@@ -2545,7 +2549,7 @@
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B114">
         <f>SUM(B113:E113)</f>
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -13757,7 +13761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
stop changer l'excel par pitié
</commit_message>
<xml_diff>
--- a/DataSeating.xlsx
+++ b/DataSeating.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m428426\Documents\Cours\Centrale\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexis\Documents\Python Scripts\ST7\Projet Air France\Projet-avion\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8223801A-300E-4578-B150-E8C5F4FDC6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="5484" activeTab="5"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="21Oct" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'26Oct'!$H$1:$H$164</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,6 +37,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -78,7 +81,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -418,19 +421,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="7" width="11.44140625" customWidth="1"/>
+    <col min="4" max="7" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -474,7 +477,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -492,7 +495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -510,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -528,7 +531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -546,7 +549,7 @@
         <v>0.22569444444444445</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -564,7 +567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -582,7 +585,7 @@
         <v>0.13194444444444445</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -602,7 +605,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -620,7 +623,7 @@
         <v>9.7222222222222224E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -638,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -658,7 +661,7 @@
         <v>0.16319444444444445</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -676,7 +679,7 @@
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -694,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -714,7 +717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -732,7 +735,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -750,7 +753,7 @@
         <v>6.5972222222222224E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -770,7 +773,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -788,7 +791,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -808,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -828,7 +831,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -848,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -866,7 +869,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -886,7 +889,7 @@
         <v>3.4722222222222224E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -906,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -924,7 +927,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -942,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2551,16 +2554,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="J91" sqref="J91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2586,7 +2589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2604,7 +2607,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2622,7 +2625,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2640,7 +2643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2676,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2694,7 +2697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2714,7 +2717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2732,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2750,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2768,7 +2771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2786,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2804,7 +2807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2822,7 +2825,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2842,7 +2845,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2862,7 +2865,7 @@
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2880,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2898,7 +2901,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2918,7 +2921,7 @@
         <v>0.37847222222222227</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2936,7 +2939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2956,7 +2959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2974,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2992,7 +2995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3010,7 +3013,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3028,7 +3031,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3064,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3456,7 +3459,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4">
@@ -3474,7 +3477,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
@@ -3492,7 +3495,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4">
@@ -3510,7 +3513,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="4">
@@ -3528,7 +3531,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="4">
@@ -3546,7 +3549,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
@@ -3566,7 +3569,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="4">
@@ -3584,7 +3587,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B56" s="4">
         <v>1</v>
@@ -3604,7 +3607,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="4">
@@ -3622,7 +3625,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4">
@@ -3640,7 +3643,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4">
@@ -3658,7 +3661,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B60" s="4">
         <v>1</v>
@@ -3676,7 +3679,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B61" s="4">
         <v>1</v>
@@ -3694,7 +3697,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B62" s="4">
         <v>1</v>
@@ -3712,7 +3715,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="4">
@@ -3730,7 +3733,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B64" s="4">
         <v>1</v>
@@ -3750,7 +3753,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B65" s="4">
         <v>1</v>
@@ -3768,7 +3771,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B66" s="4">
         <v>1</v>
@@ -3786,7 +3789,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B67" s="4">
         <v>1</v>
@@ -3804,7 +3807,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B68" s="4">
         <v>1</v>
@@ -3822,7 +3825,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4">
@@ -3840,7 +3843,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B70" s="4">
         <v>1</v>
@@ -3858,7 +3861,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B71" s="4">
         <v>1</v>
@@ -3876,7 +3879,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B72" s="4">
         <v>1</v>
@@ -3894,7 +3897,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="4">
@@ -3912,7 +3915,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B74" s="4">
         <v>1</v>
@@ -3930,7 +3933,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B75" s="4">
         <v>1</v>
@@ -3948,7 +3951,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4">
@@ -3966,7 +3969,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="4">
@@ -3984,7 +3987,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B78" s="4">
         <v>1</v>
@@ -4002,7 +4005,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B79" s="4">
         <v>1</v>
@@ -4020,7 +4023,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="4">
@@ -4038,7 +4041,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="4">
@@ -4056,7 +4059,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="4">
@@ -4074,7 +4077,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B83" s="4">
         <v>1</v>
@@ -4094,7 +4097,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B84" s="4">
         <v>1</v>
@@ -4114,7 +4117,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="4">
@@ -4132,7 +4135,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="4">
@@ -4150,7 +4153,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B87" s="4">
         <v>1</v>
@@ -4168,7 +4171,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B88" s="4">
         <v>1</v>
@@ -4188,7 +4191,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B89" s="4">
         <v>1</v>
@@ -4206,7 +4209,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="4">
@@ -4224,7 +4227,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B91" s="4">
         <v>1</v>
@@ -4242,7 +4245,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="4">
@@ -4260,7 +4263,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B93" s="4">
         <v>1</v>
@@ -4278,7 +4281,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4">
@@ -4296,7 +4299,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B95" s="4">
         <v>1</v>
@@ -4314,7 +4317,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B96" s="4">
         <v>1</v>
@@ -4364,19 +4367,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4402,7 +4405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4420,7 +4423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -4438,7 +4441,7 @@
         <v>9.7222222222222224E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4458,7 +4461,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4476,7 +4479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4494,7 +4497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4514,7 +4517,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4532,7 +4535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4550,7 +4553,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4568,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4586,7 +4589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4604,7 +4607,7 @@
         <v>9.0277777777777776E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4622,7 +4625,7 @@
         <v>9.0277777777777776E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4640,7 +4643,7 @@
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4660,7 +4663,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -4678,7 +4681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -4696,7 +4699,7 @@
         <v>9.7222222222222224E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -4714,7 +4717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4732,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -4750,7 +4753,7 @@
         <v>9.375E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4768,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -4786,7 +4789,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -4804,7 +4807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -4822,7 +4825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -4840,7 +4843,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -4858,7 +4861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -4876,7 +4879,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -6652,19 +6655,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11.44140625" style="5"/>
+    <col min="8" max="8" width="11.453125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6690,7 +6693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -6712,7 +6715,7 @@
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -6732,7 +6735,7 @@
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -6752,7 +6755,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -6774,7 +6777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -6792,7 +6795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -6810,7 +6813,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -6828,7 +6831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -6846,7 +6849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -6866,7 +6869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -6888,7 +6891,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -6906,7 +6909,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -6928,7 +6931,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -6946,7 +6949,7 @@
         <v>6.5972222222222224E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -6964,7 +6967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -6982,7 +6985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -7000,7 +7003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -7018,7 +7021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -7036,7 +7039,7 @@
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -7054,7 +7057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -7074,7 +7077,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -7092,7 +7095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -7110,7 +7113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -7128,7 +7131,7 @@
         <v>0.30902777777777779</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -7146,7 +7149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -7164,7 +7167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -7182,7 +7185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -8422,16 +8425,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8457,7 +8460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -8477,7 +8480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -8497,7 +8500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -8515,7 +8518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -8535,7 +8538,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -8553,7 +8556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -8571,7 +8574,7 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -8589,7 +8592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -8611,7 +8614,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -8633,7 +8636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -8651,7 +8654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -8669,7 +8672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -8687,7 +8690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8707,7 +8710,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -8725,7 +8728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -8743,7 +8746,7 @@
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -8761,7 +8764,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -8779,7 +8782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -8797,7 +8800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -8815,7 +8818,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -8833,7 +8836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -8851,7 +8854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -8873,7 +8876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -8891,7 +8894,7 @@
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -8909,7 +8912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -8929,7 +8932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -8947,7 +8950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -10052,22 +10055,22 @@
       <c r="H87" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="H1:H164"/>
+  <autoFilter ref="H1:H164" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10093,7 +10096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -10115,7 +10118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -10133,7 +10136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -10153,7 +10156,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -10171,7 +10174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -10189,7 +10192,7 @@
         <v>7.9861111111111105E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -10209,7 +10212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -10229,7 +10232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -10247,7 +10250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -10265,7 +10268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -10285,7 +10288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -10305,7 +10308,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -10323,7 +10326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -10341,7 +10344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -10359,7 +10362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -10377,7 +10380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -10395,7 +10398,7 @@
         <v>0.17708333333333334</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -10415,7 +10418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -10435,7 +10438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -10455,7 +10458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -10473,7 +10476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -10491,7 +10494,7 @@
         <v>7.9861111111111105E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -10509,7 +10512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -10527,7 +10530,7 @@
         <v>0.11458333333333333</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -10545,7 +10548,7 @@
         <v>7.9861111111111105E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -10563,7 +10566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -10581,7 +10584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -10599,7 +10602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -10617,7 +10620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -10635,7 +10638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -11583,16 +11586,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11618,7 +11621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -11640,7 +11643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -11658,7 +11661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -11678,7 +11681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -11696,7 +11699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -11714,7 +11717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -11734,7 +11737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -11754,7 +11757,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -11772,7 +11775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -11790,7 +11793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -11808,7 +11811,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -11826,7 +11829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -11844,7 +11847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -11862,7 +11865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -11880,7 +11883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -11898,7 +11901,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -11916,7 +11919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -11936,7 +11939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -11954,7 +11957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -11972,7 +11975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -11990,7 +11993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -12012,7 +12015,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -12032,7 +12035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -12050,7 +12053,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -12068,7 +12071,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -12086,7 +12089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -12106,7 +12109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -12124,7 +12127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -12142,7 +12145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -12160,7 +12163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -12178,7 +12181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -12196,7 +12199,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -12214,7 +12217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -12232,7 +12235,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -12250,7 +12253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -12268,7 +12271,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -12286,7 +12289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -12304,7 +12307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -12322,7 +12325,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -12340,7 +12343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -12358,7 +12361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -12376,7 +12379,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -12394,7 +12397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -12412,7 +12415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -12430,7 +12433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -12448,7 +12451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -12466,7 +12469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -12484,7 +12487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -12502,7 +12505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -12522,7 +12525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -12544,7 +12547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -12564,7 +12567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -12582,7 +12585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -12600,7 +12603,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -12618,7 +12621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -12636,7 +12639,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -12654,7 +12657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B58">
         <f>SUM(B2:B57)</f>
         <v>13</v>
@@ -12676,7 +12679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B59">
         <f>SUM(B58:E58)</f>
         <v>137</v>
@@ -12688,16 +12691,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="E57" sqref="E57:G58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12723,7 +12726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -12745,7 +12748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -12763,7 +12766,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -12783,7 +12786,7 @@
         <v>0.11458333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -12805,7 +12808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -12823,7 +12826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -12843,7 +12846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -12863,7 +12866,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -12881,7 +12884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -12901,7 +12904,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -12919,7 +12922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -12937,7 +12940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -12955,7 +12958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -12973,7 +12976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -12991,7 +12994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -13009,7 +13012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -13027,7 +13030,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -13045,7 +13048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -13065,7 +13068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -13083,7 +13086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -13103,7 +13106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -13121,7 +13124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -13139,7 +13142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -13159,7 +13162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -13179,7 +13182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -13195,7 +13198,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -13213,7 +13216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -13231,7 +13234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -13249,7 +13252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -13267,7 +13270,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -13287,7 +13290,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -13309,7 +13312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -13327,7 +13330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -13345,7 +13348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -13365,7 +13368,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -13385,7 +13388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -13403,7 +13406,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -13421,7 +13424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -13439,7 +13442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -13459,7 +13462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -13479,7 +13482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -13497,7 +13500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -13515,7 +13518,7 @@
         <v>0.11458333333333333</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -13533,7 +13536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -13551,7 +13554,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -13569,7 +13572,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -13591,7 +13594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -13609,7 +13612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -13627,7 +13630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -13645,7 +13648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -13663,7 +13666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -13681,7 +13684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -13699,7 +13702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -13717,7 +13720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B55">
         <f>SUM(B2:B54)</f>
         <v>42</v>
@@ -13739,7 +13742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B56">
         <f>SUM(B55:E55)</f>
         <v>96</v>
@@ -13751,16 +13754,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13786,7 +13789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -13804,7 +13807,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -13822,7 +13825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -13840,7 +13843,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -13860,7 +13863,7 @@
         <v>0.13541666666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -13878,7 +13881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -13896,7 +13899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -13914,7 +13917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -13934,7 +13937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -13952,7 +13955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -13970,7 +13973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -13990,7 +13993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -14008,7 +14011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -14028,7 +14031,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -14048,7 +14051,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -14066,7 +14069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -14084,7 +14087,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -14104,7 +14107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -14122,7 +14125,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -14140,7 +14143,7 @@
         <v>0.13541666666666666</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -14158,7 +14161,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -14176,7 +14179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -14194,7 +14197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -14216,7 +14219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -14234,7 +14237,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -14252,7 +14255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -14272,7 +14275,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -14292,7 +14295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -14310,7 +14313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -14328,7 +14331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -14346,7 +14349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -14364,7 +14367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -14382,7 +14385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -14400,7 +14403,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -14418,7 +14421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -14436,7 +14439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -14456,7 +14459,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -14474,7 +14477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -14494,7 +14497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -14514,7 +14517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -14532,7 +14535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -14550,7 +14553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -14570,7 +14573,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -14588,7 +14591,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -14606,7 +14609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -14624,7 +14627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -14642,7 +14645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -14660,7 +14663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -14678,7 +14681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -14696,7 +14699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -14714,7 +14717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -14734,7 +14737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -14752,7 +14755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -14770,7 +14773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -14788,7 +14791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -14806,7 +14809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -14824,7 +14827,7 @@
         <v>0.13541666666666666</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -14846,7 +14849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -14864,7 +14867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -14882,7 +14885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -14900,7 +14903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -14918,7 +14921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -14936,7 +14939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -14954,7 +14957,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -14972,7 +14975,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -14992,7 +14995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -15010,7 +15013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -15030,7 +15033,7 @@
         <v>0.13541666666666666</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -15048,7 +15051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -15066,7 +15069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -15084,7 +15087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -15102,7 +15105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -15120,7 +15123,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -15140,7 +15143,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -15160,7 +15163,7 @@
         <v>0.13541666666666666</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -15180,7 +15183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -15200,7 +15203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -15218,7 +15221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -15236,7 +15239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -15254,7 +15257,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -15272,7 +15275,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -15292,7 +15295,7 @@
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -15312,7 +15315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -15332,7 +15335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -15350,7 +15353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -15368,7 +15371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -15388,7 +15391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -15406,7 +15409,7 @@
         <v>0.13541666666666666</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -15426,7 +15429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -15446,7 +15449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B91">
         <f>SUM(B2:B90)</f>
         <v>69</v>
@@ -15468,7 +15471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B92">
         <f>SUM(B91:E91)</f>
         <v>158</v>

</xml_diff>